<commit_message>
added drools rules added costsheet xsl
</commit_message>
<xml_diff>
--- a/acm/rules/drools-costsheet-rules.xlsx
+++ b/acm/rules/drools-costsheet-rules.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjan.trifunov\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivana.shekerova\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D1C3A5B6-97EB-48D0-AFB5-32DCA7538C2F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="111"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>RuleSet</t>
   </si>
@@ -137,11 +138,20 @@
   <si>
     <t>setCostsheetNumber, dateFormat('yyyyMMdd') + '_' + $acmCostsheet.getId()</t>
   </si>
+  <si>
+    <t>Assign Alfresco Folder</t>
+  </si>
+  <si>
+    <t>container?.folder?.cmisFolderId == null</t>
+  </si>
+  <si>
+    <t>setEcmFolderPath, '/Sites/acm/documentLibrary/Expenses/' + dateFormat('yyyyMMdd') + '_' + $acmCostsheet.getId()</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -805,11 +815,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,7 +827,7 @@
     <col min="1" max="1" width="19.42578125"/>
     <col min="2" max="2" width="24.28515625"/>
     <col min="3" max="3" width="50.140625"/>
-    <col min="4" max="4" width="100.42578125"/>
+    <col min="4" max="4" width="116" customWidth="1"/>
     <col min="5" max="5" width="27.7109375"/>
     <col min="6" max="1025" width="8.7109375"/>
   </cols>
@@ -1026,9 +1036,15 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="17"/>
+      <c r="B23" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
@@ -1097,7 +1113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -1113,7 +1129,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>

</xml_diff>